<commit_message>
heuristic fixed, direction arrows added
</commit_message>
<xml_diff>
--- a/data/istanbul_anadolu_duzeltilmis-2.xlsx
+++ b/data/istanbul_anadolu_duzeltilmis-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selimsidan/Desktop/grad_project/Route_Optimization_DSS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B26FE1B-47FC-D845-8F4E-12BC88E0F22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FE4577-FF6D-D944-8178-4AE79B527A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -530,7 +530,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -839,7 +839,7 @@
         <v>40</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -931,7 +931,7 @@
         <v>40</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1000,7 +1000,7 @@
         <v>40</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>